<commit_message>
Add Python Excel tests
</commit_message>
<xml_diff>
--- a/Office-Hours/Excel-Python/report.xlsx
+++ b/Office-Hours/Excel-Python/report.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,35 +443,53 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>B1</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>C1</t>
+          <t>Grade</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A2</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>B2</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>C2</t>
-        </is>
+          <t>Tom</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Oscar</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Jay</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>